<commit_message>
Add new consistent cdfgrid analysis to SM_Main plot
</commit_message>
<xml_diff>
--- a/StanfordMuseum/Main/SM_Main.xlsx
+++ b/StanfordMuseum/Main/SM_Main.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t>Filename</t>
   </si>
@@ -296,6 +296,60 @@
   </si>
   <si>
     <t>D:\GIT\PNEE-data\StanfordMuseum\Main\pvoxNoInt\StanfordMuseum_pvox_ps32000_t28539_icdf-0_pc96000k_mc0.1_Vox96_44670.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\PNEE-data\StanfordMuseum\Main\power\StanfordMuseum_pow_ps1_t0_14354.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\PNEE-data\StanfordMuseum\Main\power\StanfordMuseum_pow_ps32000_t28319_77303.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\PNEE-data\StanfordMuseum\Main\pvox96\StanfordMuseum_pvox_ps1_t46_icdf-1_pc96000k_mc0.1_Vox96_13851.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\PNEE-data\StanfordMuseum\Main\pvox96\StanfordMuseum_pvox_ps2_t48_icdf-1_pc96000k_mc0.1_Vox96_13904.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\PNEE-data\StanfordMuseum\Main\pvox96\StanfordMuseum_pvox_ps4_t50_icdf-1_pc96000k_mc0.1_Vox96_13957.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\PNEE-data\StanfordMuseum\Main\pvox96\StanfordMuseum_pvox_ps8_t54_icdf-1_pc96000k_mc0.1_Vox96_14015.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\PNEE-data\StanfordMuseum\Main\pvox96\StanfordMuseum_pvox_ps16_t66_icdf-1_pc96000k_mc0.1_Vox96_14084.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\PNEE-data\StanfordMuseum\Main\pvox96\StanfordMuseum_pvox_ps32_t86_icdf-1_pc96000k_mc0.1_Vox96_14173.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\PNEE-data\StanfordMuseum\Main\pvox96\StanfordMuseum_pvox_ps64_t128_icdf-1_pc96000k_mc0.1_Vox96_14305.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\PNEE-data\StanfordMuseum\Main\pvox96\StanfordMuseum_pvox_ps128_t213_icdf-1_pc96000k_mc0.1_Vox96_14522.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\PNEE-data\StanfordMuseum\Main\pvox96\StanfordMuseum_pvox_ps256_t380_icdf-1_pc96000k_mc0.1_Vox96_14906.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\PNEE-data\StanfordMuseum\Main\pvox96\StanfordMuseum_pvox_ps512_t712_icdf-1_pc96000k_mc0.1_Vox96_15622.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\PNEE-data\StanfordMuseum\Main\pvox96\StanfordMuseum_pvox_ps1024_t1378_icdf-1_pc96000k_mc0.1_Vox96_17007.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\PNEE-data\StanfordMuseum\Main\pvox96\StanfordMuseum_pvox_ps2048_t2721_icdf-1_pc96000k_mc0.1_Vox96_19737.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\PNEE-data\StanfordMuseum\Main\pvox96\StanfordMuseum_pvox_ps4096_t5391_icdf-1_pc96000k_mc0.1_Vox96_25134.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\PNEE-data\StanfordMuseum\Main\pvox96\StanfordMuseum_pvox_ps8000_t10498_icdf-1_pc96000k_mc0.1_Vox96_35637.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\PNEE-data\StanfordMuseum\Main\pvox96\StanfordMuseum_pvox_ps16000_t21002_icdf-1_pc96000k_mc0.1_Vox96_56645.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\PNEE-data\StanfordMuseum\Main\pvox96\StanfordMuseum_pvox_ps32000_t42315_icdf-1_pc96000k_mc0.1_Vox96_48979.exr</t>
   </si>
 </sst>
 </file>
@@ -522,6 +576,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
@@ -573,47 +630,50 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>162.50191604501629</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>160.50146910000001</c:v>
+                  <c:v>160.501469075362</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>117.48472870000001</c:v>
+                  <c:v>117.48472871210519</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>86.605462149999994</c:v>
+                  <c:v>86.605462153385815</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>68.892218779999993</c:v>
+                  <c:v>68.89221877774969</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>46.42452875</c:v>
+                  <c:v>46.424528752479183</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33.675171550000002</c:v>
+                  <c:v>33.675171546795262</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23.06655666</c:v>
+                  <c:v>23.066556662880021</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17.369983170000001</c:v>
+                  <c:v>17.369983168650581</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12.275859730000001</c:v>
+                  <c:v>12.275859734309471</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.259694112</c:v>
+                  <c:v>8.2596941118132499</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.5289299380000001</c:v>
+                  <c:v>5.5289299376673764</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.233109775</c:v>
+                  <c:v>4.2331097754847526</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.8855106990000001</c:v>
+                  <c:v>5.8855106986990284</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.6764020390000001</c:v>
+                  <c:v>3.6764020391615602</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -640,7 +700,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$D$37:$D$52</c:f>
+              <c:f>Tabelle1!$D$38:$D$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -697,7 +757,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$37:$C$52</c:f>
+              <c:f>Tabelle1!$C$38:$C$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -774,7 +834,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$D$54:$D$69</c:f>
+              <c:f>Tabelle1!$D$55:$D$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -831,7 +891,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$54:$C$69</c:f>
+              <c:f>Tabelle1!$C$55:$C$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -908,7 +968,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$D$71:$D$86</c:f>
+              <c:f>Tabelle1!$D$72:$D$87</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -965,7 +1025,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$71:$C$86</c:f>
+              <c:f>Tabelle1!$C$72:$C$87</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1030,11 +1090,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="588112104"/>
-        <c:axId val="588110928"/>
+        <c:axId val="708462832"/>
+        <c:axId val="708457736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="588112104"/>
+        <c:axId val="708462832"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1078,12 +1138,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="588110928"/>
+        <c:crossAx val="708457736"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="588110928"/>
+        <c:axId val="708457736"/>
         <c:scaling>
           <c:logBase val="4"/>
           <c:orientation val="minMax"/>
@@ -1127,7 +1187,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="588112104"/>
+        <c:crossAx val="708462832"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1141,7 +1201,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1246,7 +1305,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -1374,7 +1445,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -1382,6 +1465,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1433,47 +1519,50 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>162.50191604501629</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>160.50146910000001</c:v>
+                  <c:v>160.501469075362</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>117.48472870000001</c:v>
+                  <c:v>117.48472871210519</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>86.605462149999994</c:v>
+                  <c:v>86.605462153385815</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>68.892218779999993</c:v>
+                  <c:v>68.89221877774969</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>46.42452875</c:v>
+                  <c:v>46.424528752479183</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33.675171550000002</c:v>
+                  <c:v>33.675171546795262</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23.06655666</c:v>
+                  <c:v>23.066556662880021</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17.369983170000001</c:v>
+                  <c:v>17.369983168650581</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12.275859730000001</c:v>
+                  <c:v>12.275859734309471</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.259694112</c:v>
+                  <c:v>8.2596941118132499</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.5289299380000001</c:v>
+                  <c:v>5.5289299376673764</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.233109775</c:v>
+                  <c:v>4.2331097754847526</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.8855106990000001</c:v>
+                  <c:v>5.8855106986990284</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.6764020390000001</c:v>
+                  <c:v>3.6764020391615602</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1496,11 +1585,23 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$D$37:$D$52</c:f>
+              <c:f>Tabelle1!$D$38:$D$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1557,7 +1658,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$37:$C$52</c:f>
+              <c:f>Tabelle1!$C$38:$C$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1630,11 +1731,23 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$D$54:$D$69</c:f>
+              <c:f>Tabelle1!$D$55:$D$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1691,7 +1804,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$54:$C$69</c:f>
+              <c:f>Tabelle1!$C$55:$C$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1764,11 +1877,23 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$D$71:$D$86</c:f>
+              <c:f>Tabelle1!$D$72:$D$87</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1825,7 +1950,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$71:$C$86</c:f>
+              <c:f>Tabelle1!$C$72:$C$87</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1890,11 +2015,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="706621144"/>
-        <c:axId val="706620360"/>
+        <c:axId val="708460872"/>
+        <c:axId val="708459304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="706621144"/>
+        <c:axId val="708460872"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1938,12 +2063,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="706620360"/>
+        <c:crossAx val="708459304"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="706620360"/>
+        <c:axId val="708459304"/>
         <c:scaling>
           <c:logBase val="4"/>
           <c:orientation val="minMax"/>
@@ -2001,7 +2126,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="706621144"/>
+        <c:crossAx val="708460872"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2021,8 +2146,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.10535643298415256"/>
           <c:y val="1.2652552926525529E-2"/>
-          <c:w val="0.77593284985226962"/>
-          <c:h val="7.1399584889995843E-2"/>
+          <c:w val="0.78942061106230699"/>
+          <c:h val="7.1544812841342537E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2129,7 +2254,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -2257,14 +2394,29 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$D$21:$D$35</c:f>
+              <c:f>Tabelle1!$D$21:$D$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2306,57 +2458,66 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>14359</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>28319</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$21:$C$35</c:f>
+              <c:f>Tabelle1!$C$21:$C$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>162.50191604501629</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>160.50146910000001</c:v>
+                  <c:v>160.501469075362</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>117.48472870000001</c:v>
+                  <c:v>117.48472871210519</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>86.605462149999994</c:v>
+                  <c:v>86.605462153385815</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>68.892218779999993</c:v>
+                  <c:v>68.89221877774969</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>46.42452875</c:v>
+                  <c:v>46.424528752479183</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33.675171550000002</c:v>
+                  <c:v>33.675171546795262</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23.06655666</c:v>
+                  <c:v>23.066556662880021</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17.369983170000001</c:v>
+                  <c:v>17.369983168650581</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12.275859730000001</c:v>
+                  <c:v>12.275859734309471</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.259694112</c:v>
+                  <c:v>8.2596941118132499</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.5289299380000001</c:v>
+                  <c:v>5.5289299376673764</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.233109775</c:v>
+                  <c:v>4.2331097754847526</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.8855106990000001</c:v>
+                  <c:v>5.8855106986990284</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.6764020390000001</c:v>
+                  <c:v>3.6764020391615602</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.655464885394681</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2379,11 +2540,23 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$D$37:$D$52</c:f>
+              <c:f>Tabelle1!$D$38:$D$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2440,7 +2613,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$37:$C$52</c:f>
+              <c:f>Tabelle1!$C$38:$C$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2513,11 +2686,23 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$D$54:$D$69</c:f>
+              <c:f>Tabelle1!$D$55:$D$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2574,7 +2759,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$54:$C$69</c:f>
+              <c:f>Tabelle1!$C$55:$C$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2647,11 +2832,23 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$D$71:$D$86</c:f>
+              <c:f>Tabelle1!$D$72:$D$87</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2708,7 +2905,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$71:$C$86</c:f>
+              <c:f>Tabelle1!$C$72:$C$87</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2759,6 +2956,152 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0.59018631899999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>pvox96</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$D$102:$D$117</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>712</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1378</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2721</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5391</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10498</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42315</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$102:$C$117</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>21.53023962</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.43277324</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.738325010000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.5569917950000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.4222706599999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.270600172</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.8741904100000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.081041157</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5509332360000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0953654239999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.87183976299999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.73035412099999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.66543866399999996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.62727514200000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.60002437799999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.59338976399999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2773,11 +3116,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="840860840"/>
-        <c:axId val="840870248"/>
+        <c:axId val="708462440"/>
+        <c:axId val="708463224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="840860840"/>
+        <c:axId val="708462440"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2821,12 +3164,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="840870248"/>
+        <c:crossAx val="708463224"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="840870248"/>
+        <c:axId val="708463224"/>
         <c:scaling>
           <c:logBase val="4"/>
           <c:orientation val="minMax"/>
@@ -2870,7 +3213,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="840860840"/>
+        <c:crossAx val="708462440"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2888,10 +3231,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="2.9062583937684454E-4"/>
-          <c:y val="0"/>
-          <c:w val="0.69104367445608372"/>
-          <c:h val="8.8269655458696542E-2"/>
+          <c:x val="5.2150108667327534E-2"/>
+          <c:y val="6.3391442155309036E-3"/>
+          <c:w val="0.67775143255506565"/>
+          <c:h val="0.11636921771466364"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4687,7 +5030,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9307500" cy="6022500"/>
+    <xdr:ext cx="9305925" cy="6010275"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1"/>
@@ -4714,7 +5057,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9307500" cy="6022500"/>
+    <xdr:ext cx="9305925" cy="6010275"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1"/>
@@ -5024,10 +5367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D99"/>
+  <dimension ref="A3:D117"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="B117" sqref="B117"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102:D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5262,15 +5605,29 @@
         <v>28317</v>
       </c>
     </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21">
+        <v>26406.872718301511</v>
+      </c>
+      <c r="C21">
+        <v>162.50191604501629</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
       <c r="B22">
-        <v>25760.721580000001</v>
+        <v>25760.721575349391</v>
       </c>
       <c r="C22">
-        <v>160.50146910000001</v>
+        <v>160.501469075362</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -5281,10 +5638,10 @@
         <v>17</v>
       </c>
       <c r="B23">
-        <v>13802.661480000001</v>
+        <v>13802.66148055695</v>
       </c>
       <c r="C23">
-        <v>117.48472870000001</v>
+        <v>117.48472871210519</v>
       </c>
       <c r="D23">
         <v>3</v>
@@ -5295,10 +5652,10 @@
         <v>18</v>
       </c>
       <c r="B24">
-        <v>7500.5060750000002</v>
+        <v>7500.506074801543</v>
       </c>
       <c r="C24">
-        <v>86.605462149999994</v>
+        <v>86.605462153385815</v>
       </c>
       <c r="D24">
         <v>7</v>
@@ -5309,10 +5666,10 @@
         <v>19</v>
       </c>
       <c r="B25">
-        <v>4746.1378080000004</v>
+        <v>4746.1378081213279</v>
       </c>
       <c r="C25">
-        <v>68.892218779999993</v>
+        <v>68.89221877774969</v>
       </c>
       <c r="D25">
         <v>14</v>
@@ -5323,10 +5680,10 @@
         <v>20</v>
       </c>
       <c r="B26">
-        <v>2155.2368700000002</v>
+        <v>2155.2368698897658</v>
       </c>
       <c r="C26">
-        <v>46.42452875</v>
+        <v>46.424528752479183</v>
       </c>
       <c r="D26">
         <v>28</v>
@@ -5337,10 +5694,10 @@
         <v>21</v>
       </c>
       <c r="B27">
-        <v>1134.0171789999999</v>
+        <v>1134.017178706089</v>
       </c>
       <c r="C27">
-        <v>33.675171550000002</v>
+        <v>33.675171546795262</v>
       </c>
       <c r="D27">
         <v>55</v>
@@ -5351,10 +5708,10 @@
         <v>22</v>
       </c>
       <c r="B28">
-        <v>532.06603629999995</v>
+        <v>532.06603628185462</v>
       </c>
       <c r="C28">
-        <v>23.06655666</v>
+        <v>23.066556662880021</v>
       </c>
       <c r="D28">
         <v>111</v>
@@ -5365,10 +5722,10 @@
         <v>23</v>
       </c>
       <c r="B29">
-        <v>301.71631530000002</v>
+        <v>301.71631527920442</v>
       </c>
       <c r="C29">
-        <v>17.369983170000001</v>
+        <v>17.369983168650581</v>
       </c>
       <c r="D29">
         <v>223</v>
@@ -5379,10 +5736,10 @@
         <v>24</v>
       </c>
       <c r="B30">
-        <v>150.69673220000001</v>
+        <v>150.69673221644061</v>
       </c>
       <c r="C30">
-        <v>12.275859730000001</v>
+        <v>12.275859734309471</v>
       </c>
       <c r="D30">
         <v>445</v>
@@ -5393,10 +5750,10 @@
         <v>25</v>
       </c>
       <c r="B31">
-        <v>68.222546820000005</v>
+        <v>68.222546820722471</v>
       </c>
       <c r="C31">
-        <v>8.259694112</v>
+        <v>8.2596941118132499</v>
       </c>
       <c r="D31">
         <v>913</v>
@@ -5407,10 +5764,10 @@
         <v>26</v>
       </c>
       <c r="B32">
-        <v>30.56906626</v>
+        <v>30.569066255634581</v>
       </c>
       <c r="C32">
-        <v>5.5289299380000001</v>
+        <v>5.5289299376673764</v>
       </c>
       <c r="D32">
         <v>1790</v>
@@ -5421,10 +5778,10 @@
         <v>27</v>
       </c>
       <c r="B33">
-        <v>17.919218369999999</v>
+        <v>17.91921837130457</v>
       </c>
       <c r="C33">
-        <v>4.233109775</v>
+        <v>4.2331097754847526</v>
       </c>
       <c r="D33">
         <v>3598</v>
@@ -5435,10 +5792,10 @@
         <v>28</v>
       </c>
       <c r="B34">
-        <v>34.639236179999997</v>
+        <v>34.63923618450071</v>
       </c>
       <c r="C34">
-        <v>5.8855106990000001</v>
+        <v>5.8855106986990284</v>
       </c>
       <c r="D34">
         <v>7186</v>
@@ -5449,853 +5806,1091 @@
         <v>29</v>
       </c>
       <c r="B35">
-        <v>13.515931950000001</v>
+        <v>13.515931953551281</v>
       </c>
       <c r="C35">
-        <v>3.6764020390000001</v>
+        <v>3.6764020391615602</v>
       </c>
       <c r="D35">
         <v>14359</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37">
-        <v>1119.8892989999999</v>
-      </c>
-      <c r="C37">
-        <v>33.464747099999997</v>
-      </c>
-      <c r="D37">
-        <v>16</v>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36">
+        <v>7.0514937575641836</v>
+      </c>
+      <c r="C36">
+        <v>2.655464885394681</v>
+      </c>
+      <c r="D36">
+        <v>28319</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B38">
-        <v>566.04254790000005</v>
+        <v>1119.8892989999999</v>
       </c>
       <c r="C38">
-        <v>23.7916487</v>
+        <v>33.464747099999997</v>
       </c>
       <c r="D38">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B39">
-        <v>279.02541789999998</v>
+        <v>566.04254790000005</v>
       </c>
       <c r="C39">
-        <v>16.704053940000001</v>
+        <v>23.7916487</v>
       </c>
       <c r="D39">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B40">
-        <v>128.47519389999999</v>
+        <v>279.02541789999998</v>
       </c>
       <c r="C40">
-        <v>11.33468985</v>
+        <v>16.704053940000001</v>
       </c>
       <c r="D40">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B41">
-        <v>59.72457464</v>
+        <v>128.47519389999999</v>
       </c>
       <c r="C41">
-        <v>7.728167612</v>
+        <v>11.33468985</v>
       </c>
       <c r="D41">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B42">
-        <v>601.68138920000001</v>
+        <v>59.72457464</v>
       </c>
       <c r="C42">
-        <v>24.529194629999999</v>
+        <v>7.728167612</v>
       </c>
       <c r="D42">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B43">
-        <v>149.5892273</v>
+        <v>601.68138920000001</v>
       </c>
       <c r="C43">
-        <v>12.23066749</v>
+        <v>24.529194629999999</v>
       </c>
       <c r="D43">
-        <v>69</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B44">
-        <v>1033.362484</v>
+        <v>149.5892273</v>
       </c>
       <c r="C44">
-        <v>32.145955950000001</v>
+        <v>12.23066749</v>
       </c>
       <c r="D44">
-        <v>125</v>
+        <v>69</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B45">
-        <v>245.5082888</v>
+        <v>1033.362484</v>
       </c>
       <c r="C45">
-        <v>15.668704119999999</v>
+        <v>32.145955950000001</v>
       </c>
       <c r="D45">
-        <v>239</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B46">
-        <v>59.800956249999999</v>
+        <v>245.5082888</v>
       </c>
       <c r="C46">
-        <v>7.7331078010000001</v>
+        <v>15.668704119999999</v>
       </c>
       <c r="D46">
-        <v>465</v>
+        <v>239</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B47">
-        <v>19.951546069999999</v>
+        <v>59.800956249999999</v>
       </c>
       <c r="C47">
-        <v>4.4667153559999999</v>
+        <v>7.7331078010000001</v>
       </c>
       <c r="D47">
-        <v>922</v>
+        <v>465</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B48">
-        <v>4.7147394599999997</v>
+        <v>19.951546069999999</v>
       </c>
       <c r="C48">
-        <v>2.1713450810000001</v>
+        <v>4.4667153559999999</v>
       </c>
       <c r="D48">
-        <v>1841</v>
+        <v>922</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B49">
-        <v>1.60852591</v>
+        <v>4.7147394599999997</v>
       </c>
       <c r="C49">
-        <v>1.2682767479999999</v>
+        <v>2.1713450810000001</v>
       </c>
       <c r="D49">
-        <v>3737</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B50">
-        <v>0.61590411499999997</v>
+        <v>1.60852591</v>
       </c>
       <c r="C50">
-        <v>0.78479558800000004</v>
+        <v>1.2682767479999999</v>
       </c>
       <c r="D50">
-        <v>7363</v>
+        <v>3737</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B51">
-        <v>1.957198692</v>
+        <v>0.61590411499999997</v>
       </c>
       <c r="C51">
-        <v>1.3989991749999999</v>
+        <v>0.78479558800000004</v>
       </c>
       <c r="D51">
-        <v>14136</v>
+        <v>7363</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52">
+        <v>1.957198692</v>
+      </c>
+      <c r="C52">
+        <v>1.3989991749999999</v>
+      </c>
+      <c r="D52">
+        <v>14136</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>76</v>
       </c>
-      <c r="B52">
+      <c r="B53">
         <v>0.534815716</v>
       </c>
-      <c r="C52">
+      <c r="C53">
         <v>0.73131095700000004</v>
       </c>
-      <c r="D52">
+      <c r="D53">
         <v>28294</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>30</v>
-      </c>
-      <c r="B54">
-        <v>964.0273702825059</v>
-      </c>
-      <c r="C54">
-        <v>31.048790158112531</v>
-      </c>
-      <c r="D54">
-        <v>21</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B55">
-        <v>512.53271711729644</v>
+        <v>964.0273702825059</v>
       </c>
       <c r="C55">
-        <v>22.639185434049889</v>
+        <v>31.048790158112531</v>
       </c>
       <c r="D55">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B56">
-        <v>262.79973127312951</v>
+        <v>512.53271711729644</v>
       </c>
       <c r="C56">
-        <v>16.211099014969019</v>
+        <v>22.639185434049889</v>
       </c>
       <c r="D56">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B57">
-        <v>118.1576210200009</v>
+        <v>262.79973127312951</v>
       </c>
       <c r="C57">
-        <v>10.87003316554282</v>
+        <v>16.211099014969019</v>
       </c>
       <c r="D57">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B58">
-        <v>54.352550654572312</v>
+        <v>118.1576210200009</v>
       </c>
       <c r="C58">
-        <v>7.3724182365471043</v>
+        <v>10.87003316554282</v>
       </c>
       <c r="D58">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B59">
-        <v>28.65762979592083</v>
+        <v>54.352550654572312</v>
       </c>
       <c r="C59">
-        <v>5.3532821517197116</v>
+        <v>7.3724182365471043</v>
       </c>
       <c r="D59">
-        <v>63</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B60">
-        <v>17.37771443106028</v>
+        <v>28.65762979592083</v>
       </c>
       <c r="C60">
-        <v>4.1686585889300503</v>
+        <v>5.3532821517197116</v>
       </c>
       <c r="D60">
-        <v>105</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B61">
-        <v>7.7981965233404544</v>
+        <v>17.37771443106028</v>
       </c>
       <c r="C61">
-        <v>2.7925251159730782</v>
+        <v>4.1686585889300503</v>
       </c>
       <c r="D61">
-        <v>189</v>
+        <v>105</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B62">
-        <v>3.7087944506806978</v>
+        <v>7.7981965233404544</v>
       </c>
       <c r="C62">
-        <v>1.9258230579886351</v>
+        <v>2.7925251159730782</v>
       </c>
       <c r="D62">
-        <v>359</v>
+        <v>189</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B63">
-        <v>1.810277892751017</v>
+        <v>3.7087944506806978</v>
       </c>
       <c r="C63">
-        <v>1.345465678771115</v>
+        <v>1.9258230579886351</v>
       </c>
       <c r="D63">
-        <v>698</v>
+        <v>359</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B64">
-        <v>1.1327491898888451</v>
+        <v>1.810277892751017</v>
       </c>
       <c r="C64">
-        <v>1.0643069058729471</v>
+        <v>1.345465678771115</v>
       </c>
       <c r="D64">
-        <v>1586</v>
+        <v>698</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B65">
-        <v>0.72411209533598953</v>
+        <v>1.1327491898888451</v>
       </c>
       <c r="C65">
-        <v>0.85094776298900365</v>
+        <v>1.0643069058729471</v>
       </c>
       <c r="D65">
-        <v>2687</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B66">
-        <v>0.55528054715626529</v>
+        <v>0.72411209533598953</v>
       </c>
       <c r="C66">
-        <v>0.74517148842146752</v>
+        <v>0.85094776298900365</v>
       </c>
       <c r="D66">
-        <v>5495</v>
+        <v>2687</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B67">
-        <v>0.43337809500642938</v>
+        <v>0.55528054715626529</v>
       </c>
       <c r="C67">
-        <v>0.65831458665779952</v>
+        <v>0.74517148842146752</v>
       </c>
       <c r="D67">
-        <v>10595</v>
+        <v>5495</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B68">
-        <v>0.40524278905542888</v>
+        <v>0.43337809500642938</v>
       </c>
       <c r="C68">
-        <v>0.63658682758554541</v>
+        <v>0.65831458665779952</v>
       </c>
       <c r="D68">
-        <v>21086</v>
+        <v>10595</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>44</v>
+      </c>
+      <c r="B69">
+        <v>0.40524278905542888</v>
+      </c>
+      <c r="C69">
+        <v>0.63658682758554541</v>
+      </c>
+      <c r="D69">
+        <v>21086</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>45</v>
       </c>
-      <c r="B69">
+      <c r="B70">
         <v>0.37577719158379091</v>
       </c>
-      <c r="C69">
+      <c r="C70">
         <v>0.61300668151643412</v>
       </c>
-      <c r="D69">
+      <c r="D70">
         <v>41862</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>77</v>
-      </c>
-      <c r="B71">
-        <v>520.18620750000002</v>
-      </c>
-      <c r="C71">
-        <v>22.807591009999999</v>
-      </c>
-      <c r="D71">
-        <v>46</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B72">
-        <v>273.19402769999999</v>
+        <v>520.18620750000002</v>
       </c>
       <c r="C72">
-        <v>16.528582140000001</v>
+        <v>22.807591009999999</v>
       </c>
       <c r="D72">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B73">
-        <v>136.57760630000001</v>
+        <v>273.19402769999999</v>
       </c>
       <c r="C73">
-        <v>11.68664222</v>
+        <v>16.528582140000001</v>
       </c>
       <c r="D73">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B74">
-        <v>64.715665670000007</v>
+        <v>136.57760630000001</v>
       </c>
       <c r="C74">
-        <v>8.044604756</v>
+        <v>11.68664222</v>
       </c>
       <c r="D74">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B75">
-        <v>32.90243212</v>
+        <v>64.715665670000007</v>
       </c>
       <c r="C75">
-        <v>5.7360641660000002</v>
+        <v>8.044604756</v>
       </c>
       <c r="D75">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B76">
-        <v>16.049475919999999</v>
+        <v>32.90243212</v>
       </c>
       <c r="C76">
-        <v>4.0061797170000002</v>
+        <v>5.7360641660000002</v>
       </c>
       <c r="D76">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B77">
-        <v>8.0820632129999996</v>
+        <v>16.049475919999999</v>
       </c>
       <c r="C77">
-        <v>2.842896976</v>
+        <v>4.0061797170000002</v>
       </c>
       <c r="D77">
-        <v>101</v>
+        <v>73</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B78">
-        <v>3.6372625080000001</v>
+        <v>8.0820632129999996</v>
       </c>
       <c r="C78">
-        <v>1.9071608499999999</v>
+        <v>2.842896976</v>
       </c>
       <c r="D78">
-        <v>159</v>
+        <v>101</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B79">
-        <v>1.6312066329999999</v>
+        <v>3.6372625080000001</v>
       </c>
       <c r="C79">
-        <v>1.2771870000000001</v>
+        <v>1.9071608499999999</v>
       </c>
       <c r="D79">
-        <v>273</v>
+        <v>159</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B80">
-        <v>0.90818302100000003</v>
+        <v>1.6312066329999999</v>
       </c>
       <c r="C80">
-        <v>0.95298636999999997</v>
+        <v>1.2771870000000001</v>
       </c>
       <c r="D80">
-        <v>503</v>
+        <v>273</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B81">
-        <v>0.60397853300000004</v>
+        <v>0.90818302100000003</v>
       </c>
       <c r="C81">
-        <v>0.77716055799999995</v>
+        <v>0.95298636999999997</v>
       </c>
       <c r="D81">
-        <v>960</v>
+        <v>503</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B82">
-        <v>0.48710620599999999</v>
+        <v>0.60397853300000004</v>
       </c>
       <c r="C82">
-        <v>0.697929943</v>
+        <v>0.77716055799999995</v>
       </c>
       <c r="D82">
-        <v>1873</v>
+        <v>960</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B83">
-        <v>0.38559722200000002</v>
+        <v>0.48710620599999999</v>
       </c>
       <c r="C83">
-        <v>0.62096475100000004</v>
+        <v>0.697929943</v>
       </c>
       <c r="D83">
-        <v>3722</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B84">
-        <v>0.35276036599999999</v>
+        <v>0.38559722200000002</v>
       </c>
       <c r="C84">
-        <v>0.59393633199999996</v>
+        <v>0.62096475100000004</v>
       </c>
       <c r="D84">
-        <v>7199</v>
+        <v>3722</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B85">
-        <v>0.34560033000000001</v>
+        <v>0.35276036599999999</v>
       </c>
       <c r="C85">
-        <v>0.58787781900000002</v>
+        <v>0.59393633199999996</v>
       </c>
       <c r="D85">
-        <v>14406</v>
+        <v>7199</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>91</v>
+      </c>
+      <c r="B86">
+        <v>0.34560033000000001</v>
+      </c>
+      <c r="C86">
+        <v>0.58787781900000002</v>
+      </c>
+      <c r="D86">
+        <v>14406</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>92</v>
       </c>
-      <c r="B86">
+      <c r="B87">
         <v>0.34831989099999999</v>
       </c>
-      <c r="C86">
+      <c r="C87">
         <v>0.59018631899999996</v>
       </c>
-      <c r="D86">
+      <c r="D87">
         <v>28539</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>4</v>
-      </c>
-      <c r="B88">
-        <v>1569.838729940117</v>
-      </c>
-      <c r="C88">
-        <v>39.621190415484961</v>
-      </c>
-      <c r="D88">
-        <v>70</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B89">
-        <v>725.81172096112084</v>
+        <v>1569.838729940117</v>
       </c>
       <c r="C89">
-        <v>26.94089309880281</v>
+        <v>39.621190415484961</v>
       </c>
       <c r="D89">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B90">
-        <v>360.18446622750542</v>
+        <v>725.81172096112084</v>
       </c>
       <c r="C90">
-        <v>18.978526450372939</v>
+        <v>26.94089309880281</v>
       </c>
       <c r="D90">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B91">
-        <v>198.1081806227206</v>
+        <v>360.18446622750542</v>
       </c>
       <c r="C91">
-        <v>14.075090785594259</v>
+        <v>18.978526450372939</v>
       </c>
       <c r="D91">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B92">
-        <v>91.989039157342546</v>
+        <v>198.1081806227206</v>
       </c>
       <c r="C92">
-        <v>9.5910916561850534</v>
+        <v>14.075090785594259</v>
       </c>
       <c r="D92">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B93">
-        <v>47.278427404231138</v>
+        <v>91.989039157342546</v>
       </c>
       <c r="C93">
-        <v>6.8759310209040887</v>
+        <v>9.5910916561850534</v>
       </c>
       <c r="D93">
-        <v>118</v>
+        <v>93</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B94">
-        <v>93.166240390720134</v>
+        <v>47.278427404231138</v>
       </c>
       <c r="C94">
-        <v>9.6522660754208456</v>
+        <v>6.8759310209040887</v>
       </c>
       <c r="D94">
-        <v>168</v>
+        <v>118</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B95">
-        <v>32.014690953992208</v>
+        <v>93.166240390720134</v>
       </c>
       <c r="C95">
-        <v>5.6581526096414372</v>
+        <v>9.6522660754208456</v>
       </c>
       <c r="D95">
-        <v>278</v>
+        <v>168</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B96">
-        <v>14.761184513885279</v>
+        <v>32.014690953992208</v>
       </c>
       <c r="C96">
-        <v>3.8420286976915312</v>
+        <v>5.6581526096414372</v>
       </c>
       <c r="D96">
-        <v>474</v>
+        <v>278</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B97">
-        <v>4.7370780299518662</v>
+        <v>14.761184513885279</v>
       </c>
       <c r="C97">
-        <v>2.1764829496120259</v>
+        <v>3.8420286976915312</v>
       </c>
       <c r="D97">
-        <v>884</v>
+        <v>474</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B98">
-        <v>3.069331559697031</v>
+        <v>4.7370780299518662</v>
       </c>
       <c r="C98">
-        <v>1.7519507868935791</v>
+        <v>2.1764829496120259</v>
       </c>
       <c r="D98">
-        <v>1667</v>
+        <v>884</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>14</v>
+      </c>
+      <c r="B99">
+        <v>3.069331559697031</v>
+      </c>
+      <c r="C99">
+        <v>1.7519507868935791</v>
+      </c>
+      <c r="D99">
+        <v>1667</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>15</v>
       </c>
-      <c r="B99">
+      <c r="B100">
         <v>1.440256533660204</v>
       </c>
-      <c r="C99">
+      <c r="C100">
         <v>1.200106884264982</v>
       </c>
-      <c r="D99">
+      <c r="D100">
         <v>3252</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>95</v>
+      </c>
+      <c r="B102">
+        <v>463.55121800000001</v>
+      </c>
+      <c r="C102">
+        <v>21.53023962</v>
+      </c>
+      <c r="D102">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>96</v>
+      </c>
+      <c r="B103">
+        <v>238.17048990000001</v>
+      </c>
+      <c r="C103">
+        <v>15.43277324</v>
+      </c>
+      <c r="D103">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>97</v>
+      </c>
+      <c r="B104">
+        <v>115.3116241</v>
+      </c>
+      <c r="C104">
+        <v>10.738325010000001</v>
+      </c>
+      <c r="D104">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>98</v>
+      </c>
+      <c r="B105">
+        <v>57.10812499</v>
+      </c>
+      <c r="C105">
+        <v>7.5569917950000001</v>
+      </c>
+      <c r="D105">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>99</v>
+      </c>
+      <c r="B106">
+        <v>29.40101911</v>
+      </c>
+      <c r="C106">
+        <v>5.4222706599999997</v>
+      </c>
+      <c r="D106">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>100</v>
+      </c>
+      <c r="B107">
+        <v>18.238025830000002</v>
+      </c>
+      <c r="C107">
+        <v>4.270600172</v>
+      </c>
+      <c r="D107">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>101</v>
+      </c>
+      <c r="B108">
+        <v>8.2609705120000001</v>
+      </c>
+      <c r="C108">
+        <v>2.8741904100000002</v>
+      </c>
+      <c r="D108">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>102</v>
+      </c>
+      <c r="B109">
+        <v>4.330732298</v>
+      </c>
+      <c r="C109">
+        <v>2.081041157</v>
+      </c>
+      <c r="D109">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>103</v>
+      </c>
+      <c r="B110">
+        <v>2.4053939020000001</v>
+      </c>
+      <c r="C110">
+        <v>1.5509332360000001</v>
+      </c>
+      <c r="D110">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>104</v>
+      </c>
+      <c r="B111">
+        <v>1.199825412</v>
+      </c>
+      <c r="C111">
+        <v>1.0953654239999999</v>
+      </c>
+      <c r="D111">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>105</v>
+      </c>
+      <c r="B112">
+        <v>0.76010457300000001</v>
+      </c>
+      <c r="C112">
+        <v>0.87183976299999999</v>
+      </c>
+      <c r="D112">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>106</v>
+      </c>
+      <c r="B113">
+        <v>0.53341714200000001</v>
+      </c>
+      <c r="C113">
+        <v>0.73035412099999997</v>
+      </c>
+      <c r="D113">
+        <v>2721</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>107</v>
+      </c>
+      <c r="B114">
+        <v>0.44280861500000002</v>
+      </c>
+      <c r="C114">
+        <v>0.66543866399999996</v>
+      </c>
+      <c r="D114">
+        <v>5391</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>108</v>
+      </c>
+      <c r="B115">
+        <v>0.39347410399999999</v>
+      </c>
+      <c r="C115">
+        <v>0.62727514200000001</v>
+      </c>
+      <c r="D115">
+        <v>10498</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>109</v>
+      </c>
+      <c r="B116">
+        <v>0.36002925400000002</v>
+      </c>
+      <c r="C116">
+        <v>0.60002437799999997</v>
+      </c>
+      <c r="D116">
+        <v>21002</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>110</v>
+      </c>
+      <c r="B117">
+        <v>0.35211141200000001</v>
+      </c>
+      <c r="C117">
+        <v>0.59338976399999999</v>
+      </c>
+      <c r="D117">
+        <v>42315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add latest ctree results to sm_main report
</commit_message>
<xml_diff>
--- a/StanfordMuseum/Main/SM_Main.xlsx
+++ b/StanfordMuseum/Main/SM_Main.xlsx
@@ -2,22 +2,23 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Diagramm3" sheetId="4" r:id="rId1"/>
     <sheet name="Diagramm4" sheetId="5" r:id="rId2"/>
-    <sheet name="Diagramm5" sheetId="6" r:id="rId3"/>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId4"/>
+    <sheet name="Diagramm5 (2)" sheetId="7" r:id="rId3"/>
+    <sheet name="Diagramm5" sheetId="6" r:id="rId4"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="127">
   <si>
     <t>Filename</t>
   </si>
@@ -350,6 +351,54 @@
   </si>
   <si>
     <t>D:\GIT\PNEE-data\StanfordMuseum\Main\pvox96\StanfordMuseum_pvox_ps32000_t42315_icdf-1_pc96000k_mc0.1_Vox96_48979.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\pbrt-v3\build\Release\images\auto_0108\photontree_main\StanfordMuseum_ptree_ps1_t188_akr_knn-1_pc96000k_nn192_mc0.1_sm0.01_13154.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\pbrt-v3\build\Release\images\auto_0108\photontree_main\StanfordMuseum_ptree_ps2_t205_akr_knn-1_pc96000k_nn192_mc0.1_sm0.01_13362.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\pbrt-v3\build\Release\images\auto_0108\photontree_main\StanfordMuseum_ptree_ps4_t226_akr_knn-1_pc96000k_nn192_mc0.1_sm0.01_13593.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\pbrt-v3\build\Release\images\auto_0108\photontree_main\StanfordMuseum_ptree_ps8_t282_akr_knn-1_pc96000k_nn192_mc0.1_sm0.01_13877.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\pbrt-v3\build\Release\images\auto_0108\photontree_main\StanfordMuseum_ptree_ps16_t377_akr_knn-1_pc96000k_nn192_mc0.1_sm0.01_14259.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\pbrt-v3\build\Release\images\auto_0108\photontree_main\StanfordMuseum_ptree_ps32_t605_akr_knn-1_pc96000k_nn192_mc0.1_sm0.01_14867.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\pbrt-v3\build\Release\images\auto_0108\photontree_main\StanfordMuseum_ptree_ps64_t1024_akr_knn-1_pc96000k_nn192_mc0.1_sm0.01_15895.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\pbrt-v3\build\Release\images\auto_0108\photontree_main\StanfordMuseum_ptree_ps128_t1826_akr_knn-1_pc96000k_nn192_mc0.1_sm0.01_17726.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\pbrt-v3\build\Release\images\auto_0108\photontree_main\StanfordMuseum_ptree_ps256_t3414_akr_knn-1_pc96000k_nn192_mc0.1_sm0.01_21145.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\pbrt-v3\build\Release\images\auto_0108\photontree_main\StanfordMuseum_ptree_ps512_t6659_akr_knn-1_pc96000k_nn192_mc0.1_sm0.01_27807.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\pbrt-v3\build\Release\images\auto_0108\photontree_main\StanfordMuseum_ptree_ps1024_t13296_akr_knn-1_pc96000k_nn192_mc0.1_sm0.01_41109.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\pbrt-v3\build\Release\images\auto_0108\photontree_main\StanfordMuseum_ptree_ps2048_t25632_akr_knn-1_pc96000k_nn192_mc0.1_sm0.01_66744.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\pbrt-v3\build\Release\images\auto_0108\photontree_main\StanfordMuseum_ptree_ps4096_t55879_akr_knn-1_pc96000k_nn192_mc0.1_sm0.01_67119.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\pbrt-v3\build\Release\images\auto_oct\cdftree_main\StanfordMuseum_ctree_ps4096_t7307_akr_knn-1_pc50000k_knc-16_cdfc-150000_mc0.1_sm0.01_pT20_5971.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\pbrt-v3\build\Release\images\auto_oct\cdftree_main\StanfordMuseum_ctree_ps8000_t14139_akr_knn-1_pc50000k_knc-16_cdfc-150000_mc0.1_sm0.01_pT20_20117.exr</t>
+  </si>
+  <si>
+    <t>D:\GIT\pbrt-v3\build\Release\images\auto_oct\cdftree_main\StanfordMuseum_ctree_ps16000_t27411_akr_knn-1_pc50000k_knc-16_cdfc-150000_mc0.1_sm0.01_pT20_22633.exr</t>
   </si>
 </sst>
 </file>
@@ -393,6 +442,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF99FF"/>
+      <color rgb="FFFF00FF"/>
+      <color rgb="FFFFCCFF"/>
+      <color rgb="FFFF66FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1090,11 +1147,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="708462832"/>
-        <c:axId val="708457736"/>
+        <c:axId val="456081616"/>
+        <c:axId val="456078872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="708462832"/>
+        <c:axId val="456081616"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1138,12 +1195,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="708457736"/>
+        <c:crossAx val="456078872"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="708457736"/>
+        <c:axId val="456078872"/>
         <c:scaling>
           <c:logBase val="4"/>
           <c:orientation val="minMax"/>
@@ -1187,7 +1244,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="708462832"/>
+        <c:crossAx val="456081616"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2015,11 +2072,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="708460872"/>
-        <c:axId val="708459304"/>
+        <c:axId val="456079656"/>
+        <c:axId val="456081224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="708460872"/>
+        <c:axId val="456079656"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2063,12 +2120,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="708459304"/>
+        <c:crossAx val="456081224"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="708459304"/>
+        <c:axId val="456081224"/>
         <c:scaling>
           <c:logBase val="4"/>
           <c:orientation val="minMax"/>
@@ -2126,7 +2183,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="708460872"/>
+        <c:crossAx val="456079656"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2247,7 +2304,301 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$E$5:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>32000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$4:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="1">
+                  <c:v>99.591218359999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74.584610740000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48.774763120000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34.891585919999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.432597619999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.912299109999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.128245160000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.7400959720000007</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.2728299610000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.1083466030000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.9470322430000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.4627388670000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.8387169179999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.98436583</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.0648641300000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Power</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$E$21:$E$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$21:$C$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>162.50191604501629</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>160.501469075362</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>117.48472871210519</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>86.605462153385815</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68.89221877774969</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>46.424528752479183</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.675171546795262</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23.066556662880021</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17.369983168650581</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.275859734309471</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.2596941118132499</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.5289299376673764</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.2331097754847526</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.8855106986990284</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.6764020391615602</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.655464885394681</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Spatial</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2258,11 +2609,942 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$E$38:$E$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$38:$C$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>33.464747099999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.7916487</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.704053940000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.33468985</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.728167612</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.529194629999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.23066749</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32.145955950000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.668704119999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.7331078010000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.4667153559999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.1713450810000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2682767479999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.78479558800000004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.3989991749999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.73131095700000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>cdfgrid no Int</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$E$72:$E$87</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$72:$C$87</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>22.807591009999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.528582140000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.68664222</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.044604756</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.7360641660000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0061797170000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.842896976</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.9071608499999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2771870000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.95298636999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.77716055799999995</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.697929943</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.62096475100000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.59393633199999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.58787781900000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.59018631899999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>cdfgrid</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$E$105:$E$120</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$105:$C$120</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>21.53023962</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.43277324</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.738325010000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.5569917950000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.4222706599999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.270600172</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.8741904100000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.081041157</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5509332360000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0953654239999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.87183976299999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.73035412099999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.66543866399999996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.62727514200000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.60002437799999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.59338976399999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>photontree</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF99FF"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF99FF"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF99FF"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$E$122:$E$134</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$122:$C$134</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>129.69573694114291</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>123.24569538380661</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>87.350973324601696</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64.86527329046416</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43.719098572931493</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30.802527748402909</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.381113083641559</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.918602451237909</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.7630586535281321</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.7783133588532536</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.7609618260288133</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.3635133758619968</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.3702158603180989</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>cdftree</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="7030A0"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$E$89:$E$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$89:$C$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>39.621190415484961</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.94089309880281</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.978526450372939</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.075090785594259</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.5910916561850534</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.8759310209040887</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.6522660754208456</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.6581526096414372</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.8420286976915312</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.1764829496120259</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.7519507868935791</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.200106884264982</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.99631316784398305</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.79182929495757937</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.71998064272519924</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="562410680"/>
+        <c:axId val="562409896"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="562410680"/>
+        <c:scaling>
+          <c:logBase val="2"/>
+          <c:orientation val="minMax"/>
+          <c:max val="33000"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+            <a:tailEnd type="triangle" w="med" len="med"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="LM Roman 12" panose="00000500000000000000" pitchFamily="50" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="562409896"/>
+        <c:crossesAt val="0.1"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="4"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="562409896"/>
+        <c:scaling>
+          <c:logBase val="4"/>
+          <c:orientation val="minMax"/>
+          <c:max val="192"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="LM Roman 12" panose="00000500000000000000" pitchFamily="50" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="562410680"/>
+        <c:crossesAt val="1"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.46839029972839885"/>
+          <c:y val="0.13100898045430534"/>
+          <c:w val="0.1685089875536285"/>
+          <c:h val="0.36993498633589977"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="LM Roman 12" panose="00000500000000000000" pitchFamily="50" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.6622401289282835E-2"/>
+          <c:y val="0.14018381070983812"/>
+          <c:w val="0.52940757453666398"/>
+          <c:h val="0.76562507264425073"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Uniform</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -2395,7 +3677,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="4"/>
+            <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
@@ -2671,154 +3953,8 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="4"/>
           <c:order val="3"/>
-          <c:tx>
-            <c:v>cdfgrid</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Tabelle1!$D$55:$D$70</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>189</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>359</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>698</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1586</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2687</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5495</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>10595</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>21086</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>41862</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Tabelle1!$C$55:$C$70</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>31.048790158112531</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>22.639185434049889</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>16.211099014969019</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10.87003316554282</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.3724182365471043</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.3532821517197116</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.1686585889300503</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.7925251159730782</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.9258230579886351</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.345465678771115</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.0643069058729471</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.85094776298900365</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.74517148842146752</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.65831458665779952</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.63658682758554541</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.61300668151643412</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
           <c:tx>
             <c:v>cdfgrid no Int</c:v>
           </c:tx>
@@ -2964,9 +4100,9 @@
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
-          <c:order val="5"/>
+          <c:order val="4"/>
           <c:tx>
-            <c:v>pvox96</c:v>
+            <c:v>cdfgrid</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -2994,7 +4130,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$D$102:$D$117</c:f>
+              <c:f>Tabelle1!$D$105:$D$120</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -3051,7 +4187,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$102:$C$117</c:f>
+              <c:f>Tabelle1!$C$105:$C$120</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -3102,6 +4238,272 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0.59338976399999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>photontree</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF99FF"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF99FF"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$D$122:$D$134</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>282</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>377</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>605</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1826</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3414</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6659</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13296</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25632</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>55879</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$122:$C$134</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>129.69573694114291</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>123.24569538380661</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>87.350973324601696</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64.86527329046416</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43.719098572931493</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30.802527748402909</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.381113083641559</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.918602451237909</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.7630586535281321</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.7783133588532536</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.7609618260288133</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.3635133758619968</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.3702158603180989</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>cdftree</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="7030A0"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$D$89:$D$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>278</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>474</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>884</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1667</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3252</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7307</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14139</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27411</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$89:$C$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>39.621190415484961</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.94089309880281</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.978526450372939</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.075090785594259</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.5910916561850534</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.8759310209040887</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.6522660754208456</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.6581526096414372</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.8420286976915312</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.1764829496120259</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.7519507868935791</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.200106884264982</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.99631316784398305</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.79182929495757937</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.71998064272519924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3116,11 +4518,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="708462440"/>
-        <c:axId val="708463224"/>
+        <c:axId val="456075736"/>
+        <c:axId val="456082400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="708462440"/>
+        <c:axId val="456075736"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3164,12 +4566,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="708463224"/>
+        <c:crossAx val="456082400"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="708463224"/>
+        <c:axId val="456082400"/>
         <c:scaling>
           <c:logBase val="4"/>
           <c:orientation val="minMax"/>
@@ -3213,7 +4615,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="708462440"/>
+        <c:crossAx val="456075736"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3231,10 +4633,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.2150108667327534E-2"/>
-          <c:y val="6.3391442155309036E-3"/>
-          <c:w val="0.67775143255506565"/>
-          <c:h val="0.11636921771466364"/>
+          <c:x val="0.46839029972839885"/>
+          <c:y val="0.13100898045430534"/>
+          <c:w val="0.1685089875536285"/>
+          <c:h val="0.36993498633589977"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3250,7 +4652,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3292,6 +4694,7 @@
       <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -3415,6 +4818,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4963,9 +6406,525 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr/>
+  <sheetPr codeName="Diagramm1"/>
   <sheetViews>
     <sheetView zoomScale="127" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
@@ -4977,7 +6936,7 @@
 
 <file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr/>
+  <sheetPr codeName="Diagramm2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4991,7 +6950,19 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Diagramm3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -5078,6 +7049,395 @@
     <xdr:clientData/>
   </xdr:absoluteAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.06994</cdr:x>
+      <cdr:y>0.07026</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.1682</cdr:x>
+      <cdr:y>0.11622</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="Textfeld 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="650875" y="422275"/>
+          <a:ext cx="914400" cy="276226"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="el-GR" sz="2000" b="0" i="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>σ</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="2000">
+            <a:latin typeface="+mn-lt"/>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.61549</cdr:x>
+      <cdr:y>0.86899</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.71375</cdr:x>
+      <cdr:y>0.94189</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="Textfeld 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5727700" y="5222875"/>
+          <a:ext cx="914400" cy="438150"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="de-DE" sz="2000">
+              <a:latin typeface="+mn-lt"/>
+            </a:rPr>
+            <a:t>ps</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9305925" cy="6010275"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.61822</cdr:x>
+      <cdr:y>0.86846</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.71648</cdr:x>
+      <cdr:y>0.94136</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="Textfeld 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5753100" y="5219700"/>
+          <a:ext cx="914400" cy="438150"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="de-DE" sz="2000">
+              <a:latin typeface="+mn-lt"/>
+            </a:rPr>
+            <a:t>s</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.06994</cdr:x>
+      <cdr:y>0.06867</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.1682</cdr:x>
+      <cdr:y>0.11463</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="Textfeld 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="650875" y="412750"/>
+          <a:ext cx="914400" cy="276226"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="el-GR" sz="2000" b="0" i="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>σ</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="2000">
+            <a:latin typeface="+mn-lt"/>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5367,10 +7727,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D117"/>
+  <sheetPr codeName="Tabelle4"/>
+  <dimension ref="A3:E134"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102:D117"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5381,7 +7742,7 @@
     <col min="4" max="4" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -5395,7 +7756,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -5408,8 +7774,11 @@
       <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -5422,8 +7791,11 @@
       <c r="D6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>60</v>
       </c>
@@ -5436,8 +7808,11 @@
       <c r="D7">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -5450,8 +7825,11 @@
       <c r="D8">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -5464,8 +7842,11 @@
       <c r="D9">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -5478,8 +7859,11 @@
       <c r="D10">
         <v>57</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -5492,8 +7876,11 @@
       <c r="D11">
         <v>114</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -5506,8 +7893,11 @@
       <c r="D12">
         <v>230</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -5520,8 +7910,11 @@
       <c r="D13">
         <v>462</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -5534,8 +7927,11 @@
       <c r="D14">
         <v>908</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -5548,8 +7944,11 @@
       <c r="D15">
         <v>1813</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -5562,8 +7961,11 @@
       <c r="D16">
         <v>3871</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -5576,8 +7978,11 @@
       <c r="D17">
         <v>7285</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -5590,8 +7995,11 @@
       <c r="D18">
         <v>14551</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -5604,8 +8012,11 @@
       <c r="D19">
         <v>28317</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>32000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>93</v>
       </c>
@@ -5618,8 +8029,11 @@
       <c r="D21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -5632,8 +8046,11 @@
       <c r="D22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -5646,8 +8063,11 @@
       <c r="D23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -5660,8 +8080,11 @@
       <c r="D24">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -5674,8 +8097,11 @@
       <c r="D25">
         <v>14</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -5688,8 +8114,11 @@
       <c r="D26">
         <v>28</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -5702,8 +8131,11 @@
       <c r="D27">
         <v>55</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -5716,8 +8148,11 @@
       <c r="D28">
         <v>111</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -5730,8 +8165,11 @@
       <c r="D29">
         <v>223</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -5744,8 +8182,11 @@
       <c r="D30">
         <v>445</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>25</v>
       </c>
@@ -5758,8 +8199,11 @@
       <c r="D31">
         <v>913</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -5772,8 +8216,11 @@
       <c r="D32">
         <v>1790</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>27</v>
       </c>
@@ -5786,8 +8233,11 @@
       <c r="D33">
         <v>3598</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -5800,8 +8250,11 @@
       <c r="D34">
         <v>7186</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -5814,8 +8267,11 @@
       <c r="D35">
         <v>14359</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>94</v>
       </c>
@@ -5828,8 +8284,11 @@
       <c r="D36">
         <v>28319</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>32000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>61</v>
       </c>
@@ -5842,8 +8301,11 @@
       <c r="D38">
         <v>16</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>62</v>
       </c>
@@ -5856,8 +8318,11 @@
       <c r="D39">
         <v>17</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>63</v>
       </c>
@@ -5870,8 +8335,11 @@
       <c r="D40">
         <v>19</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>64</v>
       </c>
@@ -5884,8 +8352,11 @@
       <c r="D41">
         <v>22</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>65</v>
       </c>
@@ -5898,8 +8369,11 @@
       <c r="D42">
         <v>29</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>66</v>
       </c>
@@ -5912,8 +8386,11 @@
       <c r="D43">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>67</v>
       </c>
@@ -5926,8 +8403,11 @@
       <c r="D44">
         <v>69</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>68</v>
       </c>
@@ -5940,8 +8420,11 @@
       <c r="D45">
         <v>125</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>69</v>
       </c>
@@ -5954,8 +8437,11 @@
       <c r="D46">
         <v>239</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>70</v>
       </c>
@@ -5968,8 +8454,11 @@
       <c r="D47">
         <v>465</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>71</v>
       </c>
@@ -5982,8 +8471,11 @@
       <c r="D48">
         <v>922</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>72</v>
       </c>
@@ -5996,8 +8488,11 @@
       <c r="D49">
         <v>1841</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>73</v>
       </c>
@@ -6010,8 +8505,11 @@
       <c r="D50">
         <v>3737</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>74</v>
       </c>
@@ -6024,8 +8522,11 @@
       <c r="D51">
         <v>7363</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>75</v>
       </c>
@@ -6038,8 +8539,11 @@
       <c r="D52">
         <v>14136</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>76</v>
       </c>
@@ -6052,8 +8556,11 @@
       <c r="D53">
         <v>28294</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <v>32000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>30</v>
       </c>
@@ -6066,8 +8573,11 @@
       <c r="D55">
         <v>21</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>31</v>
       </c>
@@ -6080,8 +8590,11 @@
       <c r="D56">
         <v>22</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>32</v>
       </c>
@@ -6094,8 +8607,11 @@
       <c r="D57">
         <v>25</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>33</v>
       </c>
@@ -6108,8 +8624,11 @@
       <c r="D58">
         <v>30</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>34</v>
       </c>
@@ -6122,8 +8641,11 @@
       <c r="D59">
         <v>41</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>35</v>
       </c>
@@ -6136,8 +8658,11 @@
       <c r="D60">
         <v>63</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>36</v>
       </c>
@@ -6150,8 +8675,11 @@
       <c r="D61">
         <v>105</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>37</v>
       </c>
@@ -6164,8 +8692,11 @@
       <c r="D62">
         <v>189</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>38</v>
       </c>
@@ -6178,8 +8709,11 @@
       <c r="D63">
         <v>359</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>39</v>
       </c>
@@ -6192,8 +8726,11 @@
       <c r="D64">
         <v>698</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>40</v>
       </c>
@@ -6206,8 +8743,11 @@
       <c r="D65">
         <v>1586</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>41</v>
       </c>
@@ -6220,8 +8760,11 @@
       <c r="D66">
         <v>2687</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>42</v>
       </c>
@@ -6234,8 +8777,11 @@
       <c r="D67">
         <v>5495</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>43</v>
       </c>
@@ -6248,8 +8794,11 @@
       <c r="D68">
         <v>10595</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68">
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>44</v>
       </c>
@@ -6262,8 +8811,11 @@
       <c r="D69">
         <v>21086</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>45</v>
       </c>
@@ -6276,8 +8828,11 @@
       <c r="D70">
         <v>41862</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <v>32000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>77</v>
       </c>
@@ -6290,8 +8845,11 @@
       <c r="D72">
         <v>46</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>78</v>
       </c>
@@ -6304,8 +8862,11 @@
       <c r="D73">
         <v>48</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>79</v>
       </c>
@@ -6318,8 +8879,11 @@
       <c r="D74">
         <v>49</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>80</v>
       </c>
@@ -6332,8 +8896,11 @@
       <c r="D75">
         <v>51</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>81</v>
       </c>
@@ -6346,8 +8913,11 @@
       <c r="D76">
         <v>59</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>82</v>
       </c>
@@ -6360,8 +8930,11 @@
       <c r="D77">
         <v>73</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>83</v>
       </c>
@@ -6374,8 +8947,11 @@
       <c r="D78">
         <v>101</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>84</v>
       </c>
@@ -6388,8 +8964,11 @@
       <c r="D79">
         <v>159</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>85</v>
       </c>
@@ -6402,8 +8981,11 @@
       <c r="D80">
         <v>273</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>86</v>
       </c>
@@ -6416,8 +8998,11 @@
       <c r="D81">
         <v>503</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>87</v>
       </c>
@@ -6430,8 +9015,11 @@
       <c r="D82">
         <v>960</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>88</v>
       </c>
@@ -6444,8 +9032,11 @@
       <c r="D83">
         <v>1873</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>89</v>
       </c>
@@ -6458,8 +9049,11 @@
       <c r="D84">
         <v>3722</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>90</v>
       </c>
@@ -6472,8 +9066,11 @@
       <c r="D85">
         <v>7199</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85">
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>91</v>
       </c>
@@ -6486,8 +9083,11 @@
       <c r="D86">
         <v>14406</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86">
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>92</v>
       </c>
@@ -6500,8 +9100,11 @@
       <c r="D87">
         <v>28539</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87">
+        <v>32000</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>4</v>
       </c>
@@ -6514,8 +9117,11 @@
       <c r="D89">
         <v>70</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>5</v>
       </c>
@@ -6528,8 +9134,11 @@
       <c r="D90">
         <v>71</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>6</v>
       </c>
@@ -6542,8 +9151,11 @@
       <c r="D91">
         <v>74</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>7</v>
       </c>
@@ -6556,8 +9168,11 @@
       <c r="D92">
         <v>80</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>8</v>
       </c>
@@ -6570,8 +9185,11 @@
       <c r="D93">
         <v>93</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>9</v>
       </c>
@@ -6584,8 +9202,11 @@
       <c r="D94">
         <v>118</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>10</v>
       </c>
@@ -6598,8 +9219,11 @@
       <c r="D95">
         <v>168</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>11</v>
       </c>
@@ -6612,8 +9236,11 @@
       <c r="D96">
         <v>278</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>12</v>
       </c>
@@ -6626,8 +9253,11 @@
       <c r="D97">
         <v>474</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>13</v>
       </c>
@@ -6640,8 +9270,11 @@
       <c r="D98">
         <v>884</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>14</v>
       </c>
@@ -6654,8 +9287,11 @@
       <c r="D99">
         <v>1667</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>15</v>
       </c>
@@ -6668,229 +9304,553 @@
       <c r="D100">
         <v>3252</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>124</v>
+      </c>
+      <c r="B101">
+        <v>0.99263992841931281</v>
+      </c>
+      <c r="C101">
+        <v>0.99631316784398305</v>
+      </c>
+      <c r="D101">
+        <v>7307</v>
+      </c>
+      <c r="E101">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>125</v>
+      </c>
+      <c r="B102">
+        <v>0.62699363235301719</v>
+      </c>
+      <c r="C102">
+        <v>0.79182929495757937</v>
+      </c>
+      <c r="D102">
+        <v>14139</v>
+      </c>
+      <c r="E102">
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>126</v>
+      </c>
+      <c r="B103">
+        <v>0.51837212589899095</v>
+      </c>
+      <c r="C103">
+        <f>SQRT(B103)</f>
+        <v>0.71998064272519924</v>
+      </c>
+      <c r="D103">
+        <v>27411</v>
+      </c>
+      <c r="E103">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>95</v>
       </c>
-      <c r="B102">
+      <c r="B105">
         <v>463.55121800000001</v>
       </c>
-      <c r="C102">
+      <c r="C105">
         <v>21.53023962</v>
       </c>
-      <c r="D102">
+      <c r="D105">
         <v>46</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="E105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>96</v>
       </c>
-      <c r="B103">
+      <c r="B106">
         <v>238.17048990000001</v>
       </c>
-      <c r="C103">
+      <c r="C106">
         <v>15.43277324</v>
       </c>
-      <c r="D103">
+      <c r="D106">
         <v>48</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+      <c r="E106">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>97</v>
       </c>
-      <c r="B104">
+      <c r="B107">
         <v>115.3116241</v>
       </c>
-      <c r="C104">
+      <c r="C107">
         <v>10.738325010000001</v>
       </c>
-      <c r="D104">
+      <c r="D107">
         <v>50</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+      <c r="E107">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>98</v>
       </c>
-      <c r="B105">
+      <c r="B108">
         <v>57.10812499</v>
       </c>
-      <c r="C105">
+      <c r="C108">
         <v>7.5569917950000001</v>
       </c>
-      <c r="D105">
+      <c r="D108">
         <v>54</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+      <c r="E108">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>99</v>
       </c>
-      <c r="B106">
+      <c r="B109">
         <v>29.40101911</v>
       </c>
-      <c r="C106">
+      <c r="C109">
         <v>5.4222706599999997</v>
       </c>
-      <c r="D106">
+      <c r="D109">
         <v>66</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+      <c r="E109">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>100</v>
       </c>
-      <c r="B107">
+      <c r="B110">
         <v>18.238025830000002</v>
       </c>
-      <c r="C107">
+      <c r="C110">
         <v>4.270600172</v>
       </c>
-      <c r="D107">
+      <c r="D110">
         <v>86</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+      <c r="E110">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>101</v>
       </c>
-      <c r="B108">
+      <c r="B111">
         <v>8.2609705120000001</v>
       </c>
-      <c r="C108">
+      <c r="C111">
         <v>2.8741904100000002</v>
       </c>
-      <c r="D108">
+      <c r="D111">
         <v>128</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+      <c r="E111">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>102</v>
       </c>
-      <c r="B109">
+      <c r="B112">
         <v>4.330732298</v>
       </c>
-      <c r="C109">
+      <c r="C112">
         <v>2.081041157</v>
       </c>
-      <c r="D109">
+      <c r="D112">
         <v>213</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+      <c r="E112">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>103</v>
       </c>
-      <c r="B110">
+      <c r="B113">
         <v>2.4053939020000001</v>
       </c>
-      <c r="C110">
+      <c r="C113">
         <v>1.5509332360000001</v>
       </c>
-      <c r="D110">
+      <c r="D113">
         <v>380</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+      <c r="E113">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>104</v>
       </c>
-      <c r="B111">
+      <c r="B114">
         <v>1.199825412</v>
       </c>
-      <c r="C111">
+      <c r="C114">
         <v>1.0953654239999999</v>
       </c>
-      <c r="D111">
+      <c r="D114">
         <v>712</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+      <c r="E114">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>105</v>
       </c>
-      <c r="B112">
+      <c r="B115">
         <v>0.76010457300000001</v>
       </c>
-      <c r="C112">
+      <c r="C115">
         <v>0.87183976299999999</v>
       </c>
-      <c r="D112">
+      <c r="D115">
         <v>1378</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+      <c r="E115">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>106</v>
       </c>
-      <c r="B113">
+      <c r="B116">
         <v>0.53341714200000001</v>
       </c>
-      <c r="C113">
+      <c r="C116">
         <v>0.73035412099999997</v>
       </c>
-      <c r="D113">
+      <c r="D116">
         <v>2721</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+      <c r="E116">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>107</v>
       </c>
-      <c r="B114">
+      <c r="B117">
         <v>0.44280861500000002</v>
       </c>
-      <c r="C114">
+      <c r="C117">
         <v>0.66543866399999996</v>
       </c>
-      <c r="D114">
+      <c r="D117">
         <v>5391</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+      <c r="E117">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>108</v>
       </c>
-      <c r="B115">
+      <c r="B118">
         <v>0.39347410399999999</v>
       </c>
-      <c r="C115">
+      <c r="C118">
         <v>0.62727514200000001</v>
       </c>
-      <c r="D115">
+      <c r="D118">
         <v>10498</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+      <c r="E118">
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>109</v>
       </c>
-      <c r="B116">
+      <c r="B119">
         <v>0.36002925400000002</v>
       </c>
-      <c r="C116">
+      <c r="C119">
         <v>0.60002437799999997</v>
       </c>
-      <c r="D116">
+      <c r="D119">
         <v>21002</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+      <c r="E119">
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>110</v>
       </c>
-      <c r="B117">
+      <c r="B120">
         <v>0.35211141200000001</v>
       </c>
-      <c r="C117">
+      <c r="C120">
         <v>0.59338976399999999</v>
       </c>
-      <c r="D117">
+      <c r="D120">
         <v>42315</v>
+      </c>
+      <c r="E120">
+        <v>32000</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>111</v>
+      </c>
+      <c r="B122">
+        <v>16820.984180706149</v>
+      </c>
+      <c r="C122">
+        <v>129.69573694114291</v>
+      </c>
+      <c r="D122">
+        <v>188</v>
+      </c>
+      <c r="E122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>112</v>
+      </c>
+      <c r="B123">
+        <v>15189.50143063804</v>
+      </c>
+      <c r="C123">
+        <v>123.24569538380661</v>
+      </c>
+      <c r="D123">
+        <v>205</v>
+      </c>
+      <c r="E123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>113</v>
+      </c>
+      <c r="B124">
+        <v>7630.1925407552781</v>
+      </c>
+      <c r="C124">
+        <v>87.350973324601696</v>
+      </c>
+      <c r="D124">
+        <v>226</v>
+      </c>
+      <c r="E124">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>114</v>
+      </c>
+      <c r="B125">
+        <v>4207.5036790466038</v>
+      </c>
+      <c r="C125">
+        <v>64.86527329046416</v>
+      </c>
+      <c r="D125">
+        <v>282</v>
+      </c>
+      <c r="E125">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>115</v>
+      </c>
+      <c r="B126">
+        <v>1911.3595800297001</v>
+      </c>
+      <c r="C126">
+        <v>43.719098572931493</v>
+      </c>
+      <c r="D126">
+        <v>377</v>
+      </c>
+      <c r="E126">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>116</v>
+      </c>
+      <c r="B127">
+        <v>948.79571569113114</v>
+      </c>
+      <c r="C127">
+        <v>30.802527748402909</v>
+      </c>
+      <c r="D127">
+        <v>605</v>
+      </c>
+      <c r="E127">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>117</v>
+      </c>
+      <c r="B128">
+        <v>457.15199669546843</v>
+      </c>
+      <c r="C128">
+        <v>21.381113083641559</v>
+      </c>
+      <c r="D128">
+        <v>1024</v>
+      </c>
+      <c r="E128">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>118</v>
+      </c>
+      <c r="B129">
+        <v>193.72749419560591</v>
+      </c>
+      <c r="C129">
+        <v>13.918602451237909</v>
+      </c>
+      <c r="D129">
+        <v>1826</v>
+      </c>
+      <c r="E129">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>119</v>
+      </c>
+      <c r="B130">
+        <v>95.317314272230547</v>
+      </c>
+      <c r="C130">
+        <v>9.7630586535281321</v>
+      </c>
+      <c r="D130">
+        <v>3414</v>
+      </c>
+      <c r="E130">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>120</v>
+      </c>
+      <c r="B131">
+        <v>45.94553199080849</v>
+      </c>
+      <c r="C131">
+        <v>6.7783133588532536</v>
+      </c>
+      <c r="D131">
+        <v>6659</v>
+      </c>
+      <c r="E131">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>121</v>
+      </c>
+      <c r="B132">
+        <v>22.666757508903611</v>
+      </c>
+      <c r="C132">
+        <v>4.7609618260288133</v>
+      </c>
+      <c r="D132">
+        <v>13296</v>
+      </c>
+      <c r="E132">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>122</v>
+      </c>
+      <c r="B133">
+        <v>11.31322222960257</v>
+      </c>
+      <c r="C133">
+        <v>3.3635133758619968</v>
+      </c>
+      <c r="D133">
+        <v>25632</v>
+      </c>
+      <c r="E133">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>123</v>
+      </c>
+      <c r="B134">
+        <v>5.6179232245034667</v>
+      </c>
+      <c r="C134">
+        <v>2.3702158603180989</v>
+      </c>
+      <c r="D134">
+        <v>55879</v>
+      </c>
+      <c r="E134">
+        <v>4096</v>
       </c>
     </row>
   </sheetData>

</xml_diff>